<commit_message>
file statistics completed and comment errors fixed
</commit_message>
<xml_diff>
--- a/file-statistics.xlsx
+++ b/file-statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\TU Darmstadt\Masterarbeit\chess-annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91D8578-5E03-4602-AB6C-0A83A115A498}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F4BB75-20DE-4649-A4A3-5A2AF4E03606}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CB797301-E421-4290-AD9C-F33B313D1461}"/>
   </bookViews>
@@ -24,8 +24,210 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Florian Beck</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{C28DEA67-3AEE-4CBA-A5B2-2F4F9CD26D73}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{0080EC2A-0D44-4C87-BF52-89EFA77136F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{40B86B38-7742-45AF-A057-C034A935BF80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+frz</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{2D463ED3-2D6E-4F83-B2D8-E735250C5B68}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{15927E8B-C4AE-4367-AEB9-72452F39AD84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{FF65F995-8B50-4EE5-B2EB-06F643D44A6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{32105AD6-B5F7-4F5F-9E18-EA223190FFB9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{14F7E778-DACF-4C1A-B94B-D2D3A8D7C6D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+multiple languages</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>files/bali02.pgn</t>
   </si>
@@ -229,19 +431,35 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,97 +502,100 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7184EF4-25C3-4BC2-8006-D03EA3E4CADA}" name="Tabelle4" displayName="Tabelle4" ref="A1:AD40" totalsRowCount="1">
-  <autoFilter ref="A1:AD39" xr:uid="{CF6BAA34-CBCC-4959-B3F2-DD4EC0EA728D}"/>
-  <tableColumns count="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7184EF4-25C3-4BC2-8006-D03EA3E4CADA}" name="Tabelle4" displayName="Tabelle4" ref="A1:AE40" totalsRowCount="1">
+  <autoFilter ref="A1:AE39" xr:uid="{CF6BAA34-CBCC-4959-B3F2-DD4EC0EA728D}"/>
+  <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{E6C94211-23A1-4145-A10C-FC15029287A1}" name="File"/>
-    <tableColumn id="2" xr3:uid="{2FB076B9-73AB-4E61-83C3-83A87CEDE980}" name="All" totalsRowFunction="custom">
-      <calculatedColumnFormula>SUM(C2:AD2)</calculatedColumnFormula>
+    <tableColumn id="31" xr3:uid="{F174BBBB-376E-4106-BA42-E7CF2824B6B0}" name="Comments" totalsRowFunction="custom">
       <totalsRowFormula>SUM(B2:B39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{65EB2F08-54D9-4E5D-B9F7-586824072F43}" name="1" totalsRowFunction="custom">
+    <tableColumn id="2" xr3:uid="{2FB076B9-73AB-4E61-83C3-83A87CEDE980}" name="All" totalsRowFunction="custom">
+      <calculatedColumnFormula>SUM(D2:AE2)</calculatedColumnFormula>
       <totalsRowFormula>SUM(C2:C39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{69006022-1908-459E-A8A6-C84B888F5F50}" name="2" totalsRowFunction="custom">
+    <tableColumn id="3" xr3:uid="{65EB2F08-54D9-4E5D-B9F7-586824072F43}" name="1" totalsRowFunction="custom">
       <totalsRowFormula>SUM(D2:D39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C3528F40-E2F3-4B3D-B1BB-925AB8DDAD15}" name="3" totalsRowFunction="custom">
+    <tableColumn id="4" xr3:uid="{69006022-1908-459E-A8A6-C84B888F5F50}" name="2" totalsRowFunction="custom">
       <totalsRowFormula>SUM(E2:E39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{760AB30D-5010-4EF1-B595-F42831A002FC}" name="4" totalsRowFunction="custom">
+    <tableColumn id="5" xr3:uid="{C3528F40-E2F3-4B3D-B1BB-925AB8DDAD15}" name="3" totalsRowFunction="custom">
       <totalsRowFormula>SUM(F2:F39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FCBBDE9E-4109-41FB-9E56-80D3E9F87C4C}" name="5" totalsRowFunction="custom">
+    <tableColumn id="6" xr3:uid="{760AB30D-5010-4EF1-B595-F42831A002FC}" name="4" totalsRowFunction="custom">
       <totalsRowFormula>SUM(G2:G39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0E9D343C-38E3-499F-843B-097F558A6C3E}" name="6" totalsRowFunction="custom">
+    <tableColumn id="7" xr3:uid="{FCBBDE9E-4109-41FB-9E56-80D3E9F87C4C}" name="5" totalsRowFunction="custom">
       <totalsRowFormula>SUM(H2:H39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A47892F-34FC-4583-A284-D4668630E858}" name="7" totalsRowFunction="custom">
+    <tableColumn id="8" xr3:uid="{0E9D343C-38E3-499F-843B-097F558A6C3E}" name="6" totalsRowFunction="custom">
       <totalsRowFormula>SUM(I2:I39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{771EA691-77BA-4D45-AE31-6FDCE135BF75}" name="8" totalsRowFunction="custom">
+    <tableColumn id="9" xr3:uid="{4A47892F-34FC-4583-A284-D4668630E858}" name="7" totalsRowFunction="custom">
       <totalsRowFormula>SUM(J2:J39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{36EE787E-EA94-4E32-A670-C7355BFDEB4D}" name="10" totalsRowFunction="custom">
+    <tableColumn id="10" xr3:uid="{771EA691-77BA-4D45-AE31-6FDCE135BF75}" name="8" totalsRowFunction="custom">
       <totalsRowFormula>SUM(K2:K39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{58911C97-3A9D-4CE9-9AFB-C4268FAAE96B}" name="11" totalsRowFunction="custom">
+    <tableColumn id="11" xr3:uid="{36EE787E-EA94-4E32-A670-C7355BFDEB4D}" name="10" totalsRowFunction="custom">
       <totalsRowFormula>SUM(L2:L39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4ED60B13-E4FB-4FFC-BA08-FB03C9FD29A5}" name="12" totalsRowFunction="custom">
+    <tableColumn id="12" xr3:uid="{58911C97-3A9D-4CE9-9AFB-C4268FAAE96B}" name="11" totalsRowFunction="custom">
       <totalsRowFormula>SUM(M2:M39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{EB91C9F1-2330-4E73-A610-1A873807035D}" name="13" totalsRowFunction="custom">
+    <tableColumn id="13" xr3:uid="{4ED60B13-E4FB-4FFC-BA08-FB03C9FD29A5}" name="12" totalsRowFunction="custom">
       <totalsRowFormula>SUM(N2:N39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{573D498E-F0E6-4E50-9260-3025FDAA1521}" name="14" totalsRowFunction="custom">
+    <tableColumn id="14" xr3:uid="{EB91C9F1-2330-4E73-A610-1A873807035D}" name="13" totalsRowFunction="custom">
       <totalsRowFormula>SUM(O2:O39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{E6DB5C83-E5DC-4947-A6E4-5F05354A6B30}" name="15" totalsRowFunction="custom">
+    <tableColumn id="15" xr3:uid="{573D498E-F0E6-4E50-9260-3025FDAA1521}" name="14" totalsRowFunction="custom">
       <totalsRowFormula>SUM(P2:P39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5A70BCB7-41A1-430D-93F1-4807BC94E4F4}" name="16" totalsRowFunction="custom">
+    <tableColumn id="16" xr3:uid="{E6DB5C83-E5DC-4947-A6E4-5F05354A6B30}" name="15" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Q2:Q39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{73CC9737-B59A-446B-9EE5-444C4C840345}" name="17" totalsRowFunction="custom">
+    <tableColumn id="17" xr3:uid="{5A70BCB7-41A1-430D-93F1-4807BC94E4F4}" name="16" totalsRowFunction="custom">
       <totalsRowFormula>SUM(R2:R39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{998CD29A-C5ED-4C95-B4A3-4E1D37190A4A}" name="18" totalsRowFunction="custom">
+    <tableColumn id="18" xr3:uid="{73CC9737-B59A-446B-9EE5-444C4C840345}" name="17" totalsRowFunction="custom">
       <totalsRowFormula>SUM(S2:S39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{3A3EE362-AC9D-40DE-AE2E-AAF1A6864D14}" name="19" totalsRowFunction="custom">
+    <tableColumn id="19" xr3:uid="{998CD29A-C5ED-4C95-B4A3-4E1D37190A4A}" name="18" totalsRowFunction="custom">
       <totalsRowFormula>SUM(T2:T39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{9BAFEC70-9B51-4DE0-819A-0D51BE216142}" name="22" totalsRowFunction="custom">
+    <tableColumn id="20" xr3:uid="{3A3EE362-AC9D-40DE-AE2E-AAF1A6864D14}" name="19" totalsRowFunction="custom">
       <totalsRowFormula>SUM(U2:U39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{8593A5D6-04A4-4FA4-8E58-A3D48B2E5AEC}" name="32" totalsRowFunction="custom">
+    <tableColumn id="21" xr3:uid="{9BAFEC70-9B51-4DE0-819A-0D51BE216142}" name="22" totalsRowFunction="custom">
       <totalsRowFormula>SUM(V2:V39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{FEB66F49-9A94-43D0-826B-41A8F6CA67F3}" name="36" totalsRowFunction="custom">
+    <tableColumn id="22" xr3:uid="{8593A5D6-04A4-4FA4-8E58-A3D48B2E5AEC}" name="32" totalsRowFunction="custom">
       <totalsRowFormula>SUM(W2:W39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{200AA973-1C41-4B84-9149-440DD05278EF}" name="40" totalsRowFunction="custom">
+    <tableColumn id="23" xr3:uid="{FEB66F49-9A94-43D0-826B-41A8F6CA67F3}" name="36" totalsRowFunction="custom">
       <totalsRowFormula>SUM(X2:X39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{14CF7637-1A32-4B5F-841B-4DCD0B59B2B4}" name="44" totalsRowFunction="custom">
+    <tableColumn id="24" xr3:uid="{200AA973-1C41-4B84-9149-440DD05278EF}" name="40" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Y2:Y39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{003DB797-6948-4270-953C-53696BD6AC59}" name="132" totalsRowFunction="custom">
+    <tableColumn id="25" xr3:uid="{14CF7637-1A32-4B5F-841B-4DCD0B59B2B4}" name="44" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Z2:Z39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{24274AE3-E617-46F0-B73F-2C42B18E618D}" name="133" totalsRowFunction="custom">
+    <tableColumn id="26" xr3:uid="{003DB797-6948-4270-953C-53696BD6AC59}" name="132" totalsRowFunction="custom">
       <totalsRowFormula>SUM(AA2:AA39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{3B64F48B-38B9-4A07-8306-1B7A70842A40}" name="138" totalsRowFunction="custom">
+    <tableColumn id="27" xr3:uid="{24274AE3-E617-46F0-B73F-2C42B18E618D}" name="133" totalsRowFunction="custom">
       <totalsRowFormula>SUM(AB2:AB39)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{B4755D5F-D63B-482A-BBDA-EEDF0D649C17}" name="142" totalsRowFunction="custom">
+    <tableColumn id="28" xr3:uid="{3B64F48B-38B9-4A07-8306-1B7A70842A40}" name="138" totalsRowFunction="custom">
       <totalsRowFormula>SUM(AC2:AC39)</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="29" xr3:uid="{B4755D5F-D63B-482A-BBDA-EEDF0D649C17}" name="142" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(AD2:AD39)</totalsRowFormula>
+    </tableColumn>
     <tableColumn id="30" xr3:uid="{F962C768-4B69-4ACA-ABB5-B35A21282D38}" name="146" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(AD2:AD39)</totalsRowFormula>
+      <totalsRowFormula>SUM(AE2:AE39)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -677,140 +898,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2754611A-D4BC-4997-8208-F8CC3E0865F3}">
-  <dimension ref="A1:AD40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2754611A-D4BC-4997-8208-F8CC3E0865F3}">
+  <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="25" width="5.140625" customWidth="1"/>
-    <col min="26" max="30" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="4" max="26" width="5.140625" customWidth="1"/>
+    <col min="27" max="31" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>65</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>52</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>55</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>58</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>SUM(C2:AD2)</f>
+        <v>456</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C10" si="0">SUM(D2:AE2)</f>
         <v>41</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>9</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
         <v>0</v>
       </c>
@@ -818,35 +1043,35 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>4</v>
       </c>
-      <c r="R2">
-        <v>2</v>
-      </c>
       <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2">
         <v>4</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>3</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
       <c r="V2">
         <v>0</v>
       </c>
@@ -874,16 +1099,19 @@
       <c r="AD2">
         <v>0</v>
       </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <f>SUM(C3:AD3)</f>
-        <v>0</v>
+        <v>939</v>
       </c>
       <c r="C3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D3">
@@ -967,69 +1195,72 @@
       <c r="AD3">
         <v>0</v>
       </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <f>SUM(C4:AD4)</f>
+        <v>554</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>53</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>5</v>
-      </c>
-      <c r="O4">
-        <v>6</v>
       </c>
       <c r="P4">
         <v>6</v>
       </c>
       <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
         <v>12</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>7</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>5</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
       <c r="U4">
         <v>0</v>
       </c>
@@ -1037,39 +1268,42 @@
         <v>0</v>
       </c>
       <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>10</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>4</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>7</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>4</v>
       </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <v>7</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <f>SUM(C5:AD5)</f>
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D5">
@@ -1153,36 +1387,39 @@
       <c r="AD5">
         <v>0</v>
       </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <f>SUM(C6:AD6)</f>
+        <v>3742</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
         <v>1263</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>382</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>230</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>40</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>285</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>305</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
@@ -1199,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1211,11 +1448,11 @@
         <v>0</v>
       </c>
       <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>3</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
       <c r="U6">
         <v>0</v>
       </c>
@@ -1246,23 +1483,26 @@
       <c r="AD6">
         <v>0</v>
       </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <f>SUM(C7:AD7)</f>
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1339,17 +1579,20 @@
       <c r="AD7">
         <v>0</v>
       </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <f>SUM(C8:AD8)</f>
-        <v>2</v>
+        <v>6276</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1382,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1397,10 +1640,10 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1432,16 +1675,19 @@
       <c r="AD8">
         <v>0</v>
       </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <f>SUM(C9:AD9)</f>
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9">
@@ -1525,36 +1771,39 @@
       <c r="AD9">
         <v>0</v>
       </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <f>SUM(C10:AD10)</f>
+        <v>201</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>37</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>5</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>5</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
@@ -1618,36 +1867,39 @@
       <c r="AD10">
         <v>0</v>
       </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B39" si="0">SUM(C11:AD11)</f>
+        <v>702</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C39" si="1">SUM(D11:AE11)</f>
         <v>228</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>86</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>44</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>12</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>43</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>18</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
       <c r="J11">
         <v>0</v>
       </c>
@@ -1655,34 +1907,34 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
         <v>3</v>
       </c>
-      <c r="R11">
-        <v>2</v>
-      </c>
       <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
         <v>4</v>
       </c>
-      <c r="T11">
-        <v>2</v>
-      </c>
       <c r="U11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1694,10 +1946,10 @@
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -1706,21 +1958,24 @@
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D12">
@@ -1804,36 +2059,39 @@
       <c r="AD12">
         <v>0</v>
       </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <v>713</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>24</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>13</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
         <v>7</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>12</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="J13">
         <v>0</v>
       </c>
@@ -1841,34 +2099,34 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>2</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1877,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -1895,37 +2153,40 @@
         <v>0</v>
       </c>
       <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <v>1085</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>69</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>15</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1990,90 +2251,93 @@
       <c r="AD14">
         <v>0</v>
       </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <v>3109</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
         <v>714</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>248</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>48</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>122</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>16</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>70</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>36</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>14</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
       <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>19</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
       <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>12</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>21</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>8</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>17</v>
       </c>
-      <c r="R15">
-        <v>2</v>
-      </c>
       <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
         <v>50</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>4</v>
       </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
       <c r="V15">
         <v>0</v>
       </c>
       <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
         <v>7</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>11</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>3</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>5</v>
       </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
       <c r="AB15">
         <v>0</v>
       </c>
@@ -2081,18 +2345,21 @@
         <v>0</v>
       </c>
       <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D16">
@@ -2176,32 +2443,35 @@
       <c r="AD16">
         <v>0</v>
       </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>3</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2269,36 +2539,39 @@
       <c r="AD17">
         <v>0</v>
       </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>6</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>3</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>32</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>20</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>9</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
       <c r="J18">
         <v>0</v>
       </c>
@@ -2306,35 +2579,35 @@
         <v>0</v>
       </c>
       <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>6</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="P18">
         <v>12</v>
       </c>
       <c r="Q18">
+        <v>12</v>
+      </c>
+      <c r="R18">
         <v>3</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>5</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>4</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>3</v>
       </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
       <c r="V18">
         <v>0</v>
       </c>
@@ -2362,33 +2635,36 @@
       <c r="AD18">
         <v>0</v>
       </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>48</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>6</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
         <v>0</v>
       </c>
@@ -2399,19 +2675,19 @@
         <v>0</v>
       </c>
       <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>3</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2423,10 +2699,10 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -2453,38 +2729,41 @@
         <v>0</v>
       </c>
       <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <v>1162</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>21</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>14</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
       <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
         <v>11</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>24</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>13</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
       <c r="J20">
         <v>0</v>
       </c>
@@ -2498,25 +2777,25 @@
         <v>0</v>
       </c>
       <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
         <v>3</v>
       </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
       <c r="P20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
         <v>5</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
       <c r="S20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -2546,38 +2825,41 @@
         <v>0</v>
       </c>
       <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <v>3946</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
         <v>885</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>570</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>149</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>60</v>
       </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
       <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
         <v>19</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>5</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
       <c r="J21">
         <v>0</v>
       </c>
@@ -2585,53 +2867,53 @@
         <v>0</v>
       </c>
       <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>10</v>
       </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
         <v>9</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>10</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>20</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>16</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>3</v>
       </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
       <c r="W21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
         <v>4</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>3</v>
       </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
       <c r="AB21">
         <v>0</v>
       </c>
@@ -2641,36 +2923,39 @@
       <c r="AD21">
         <v>0</v>
       </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>43</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>6</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>14</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>6</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
       <c r="J22">
         <v>0</v>
       </c>
@@ -2702,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -2734,33 +3019,36 @@
       <c r="AD22">
         <v>0</v>
       </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <v>7056</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>9</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
         <v>3</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
         <v>0</v>
       </c>
@@ -2783,10 +3071,10 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23">
         <v>0</v>
@@ -2795,10 +3083,10 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -2827,44 +3115,47 @@
       <c r="AD23">
         <v>0</v>
       </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <v>4913</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
         <v>206</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>138</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>32</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>11</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
       <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>11</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2879,17 +3170,17 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
         <v>5</v>
       </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
       <c r="U24">
         <v>0</v>
       </c>
@@ -2920,36 +3211,39 @@
       <c r="AD24">
         <v>0</v>
       </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <v>453</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
         <v>166</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>20</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>17</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>7</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>37</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>32</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>8</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
       <c r="J25">
         <v>0</v>
       </c>
@@ -2957,35 +3251,35 @@
         <v>0</v>
       </c>
       <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>11</v>
       </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P25">
         <v>8</v>
       </c>
       <c r="Q25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="R25">
         <v>3</v>
       </c>
       <c r="S25">
+        <v>3</v>
+      </c>
+      <c r="T25">
         <v>8</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>4</v>
       </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
       <c r="V25">
         <v>0</v>
       </c>
@@ -3013,35 +3307,38 @@
       <c r="AD25">
         <v>0</v>
       </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>13</v>
       </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
       <c r="E26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
         <v>3</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>11</v>
       </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
       <c r="I26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -3050,32 +3347,32 @@
         <v>0</v>
       </c>
       <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>7</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
       <c r="N26">
         <v>0</v>
       </c>
       <c r="O26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>3</v>
       </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
       <c r="U26">
         <v>0</v>
       </c>
@@ -3098,28 +3395,31 @@
         <v>0</v>
       </c>
       <c r="AB26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3128,10 +3428,10 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -3152,25 +3452,25 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27">
         <v>0</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -3199,71 +3499,74 @@
       <c r="AD27">
         <v>0</v>
       </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <v>472</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>20</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>7</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>17</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>3</v>
       </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
       <c r="J28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <v>3</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>5</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>14</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>5</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>15</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>3</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>4</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
       <c r="U28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -3272,103 +3575,106 @@
         <v>0</v>
       </c>
       <c r="X28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z28">
         <v>0</v>
       </c>
       <c r="AA28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC28">
         <v>0</v>
       </c>
       <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <v>779</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>48</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>7</v>
       </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
       <c r="F29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>11</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>4</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
       <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
         <v>5</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29">
         <v>5</v>
       </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
       <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
         <v>6</v>
       </c>
-      <c r="R29">
-        <v>2</v>
-      </c>
       <c r="S29">
+        <v>2</v>
+      </c>
+      <c r="T29">
         <v>3</v>
       </c>
-      <c r="T29">
-        <v>2</v>
-      </c>
       <c r="U29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V29">
         <v>0</v>
       </c>
       <c r="W29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z29">
         <v>0</v>
@@ -3377,44 +3683,47 @@
         <v>0</v>
       </c>
       <c r="AB29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <v>1326</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
         <v>188</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>73</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>31</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>10</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>8</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>28</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>27</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
       <c r="J30">
         <v>0</v>
       </c>
@@ -3422,34 +3731,34 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
         <v>4</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
       <c r="Q30">
         <v>0</v>
       </c>
       <c r="R30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -3476,23 +3785,26 @@
         <v>0</v>
       </c>
       <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <v>298</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>54</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
       <c r="E31">
         <v>0</v>
       </c>
@@ -3571,29 +3883,32 @@
       <c r="AD31">
         <v>0</v>
       </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <v>572</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -3632,10 +3947,10 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -3647,10 +3962,10 @@
         <v>0</v>
       </c>
       <c r="Y32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA32">
         <v>0</v>
@@ -3664,36 +3979,39 @@
       <c r="AD32">
         <v>0</v>
       </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <v>681</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>10</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>13</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>15</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>8</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
       <c r="J33">
         <v>0</v>
       </c>
@@ -3701,34 +4019,34 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
         <v>4</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>3</v>
       </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
       <c r="T33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -3757,221 +4075,230 @@
       <c r="AD33">
         <v>0</v>
       </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
         <v>173</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>45</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>5</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>3</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
       <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>13</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>10</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
       <c r="J34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
         <v>7</v>
       </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
       <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
         <v>11</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>15</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>7</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>14</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>7</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>9</v>
       </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
       <c r="U34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34">
         <v>0</v>
       </c>
       <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
         <v>4</v>
       </c>
-      <c r="X34">
-        <v>2</v>
-      </c>
       <c r="Y34">
+        <v>2</v>
+      </c>
+      <c r="Z34">
         <v>3</v>
       </c>
-      <c r="Z34">
+      <c r="AA34">
         <v>12</v>
       </c>
-      <c r="AA34">
-        <v>0</v>
-      </c>
       <c r="AB34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <v>593</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
         <v>237</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>69</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>10</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
       <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <v>3</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>43</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>13</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
       <c r="J35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
         <v>11</v>
       </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
       <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
         <v>9</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>14</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>3</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>14</v>
       </c>
-      <c r="R35">
-        <v>2</v>
-      </c>
       <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
         <v>10</v>
       </c>
-      <c r="T35">
-        <v>2</v>
-      </c>
       <c r="U35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V35">
         <v>0</v>
       </c>
       <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
         <v>9</v>
       </c>
-      <c r="X35">
+      <c r="Y35">
         <v>4</v>
       </c>
-      <c r="Y35">
-        <v>2</v>
-      </c>
       <c r="Z35">
+        <v>2</v>
+      </c>
+      <c r="AA35">
         <v>12</v>
       </c>
-      <c r="AA35">
-        <v>0</v>
-      </c>
       <c r="AB35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
         <v>147</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>21</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>4</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>5</v>
       </c>
-      <c r="F36">
-        <v>2</v>
-      </c>
       <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
         <v>16</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -3980,53 +4307,53 @@
         <v>0</v>
       </c>
       <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
         <v>4</v>
       </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
       <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
         <v>14</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>6</v>
       </c>
-      <c r="P36">
-        <v>1</v>
-      </c>
       <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
         <v>14</v>
       </c>
-      <c r="R36">
+      <c r="S36">
         <v>5</v>
       </c>
-      <c r="S36">
+      <c r="T36">
         <v>29</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>5</v>
       </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
       <c r="V36">
         <v>0</v>
       </c>
       <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
         <v>3</v>
       </c>
-      <c r="X36">
+      <c r="Y36">
         <v>6</v>
       </c>
-      <c r="Y36">
+      <c r="Z36">
         <v>8</v>
       </c>
-      <c r="Z36">
+      <c r="AA36">
         <v>3</v>
       </c>
-      <c r="AA36">
-        <v>0</v>
-      </c>
       <c r="AB36">
         <v>0</v>
       </c>
@@ -4036,36 +4363,39 @@
       <c r="AD36">
         <v>0</v>
       </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <v>914</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
         <v>251</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>30</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>13</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>4</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>3</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>19</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>15</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
       <c r="J37">
         <v>0</v>
       </c>
@@ -4073,35 +4403,35 @@
         <v>0</v>
       </c>
       <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
         <v>53</v>
       </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
       <c r="N37">
         <v>0</v>
       </c>
       <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
         <v>31</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>10</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>27</v>
       </c>
-      <c r="R37">
+      <c r="S37">
         <v>14</v>
       </c>
-      <c r="S37">
+      <c r="T37">
         <v>16</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>15</v>
       </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
       <c r="V37">
         <v>0</v>
       </c>
@@ -4124,49 +4454,52 @@
         <v>0</v>
       </c>
       <c r="AC37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD37">
+        <v>1</v>
+      </c>
+      <c r="AE37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <v>374</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>36</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>8</v>
       </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
       <c r="F38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
         <v>3</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -4175,10 +4508,10 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -4187,11 +4520,11 @@
         <v>0</v>
       </c>
       <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
         <v>3</v>
       </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
       <c r="U38">
         <v>0</v>
       </c>
@@ -4222,36 +4555,39 @@
       <c r="AD38">
         <v>0</v>
       </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <v>6850</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
         <v>1755</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>1022</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>224</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>23</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>28</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>199</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>175</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
       <c r="J39">
         <v>0</v>
       </c>
@@ -4259,35 +4595,35 @@
         <v>0</v>
       </c>
       <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
         <v>42</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
       <c r="N39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P39">
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
         <v>20</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>19</v>
       </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
       <c r="V39">
         <v>0</v>
       </c>
@@ -4315,129 +4651,137 @@
       <c r="AD39">
         <v>0</v>
       </c>
+      <c r="AE39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B40">
         <f>SUM(B2:B39)</f>
-        <v>7482</v>
+        <v>50762</v>
       </c>
       <c r="C40">
         <f>SUM(C2:C39)</f>
+        <v>7482</v>
+      </c>
+      <c r="D40">
+        <f>SUM(D2:D39)</f>
         <v>3225</v>
       </c>
-      <c r="D40">
-        <f t="shared" ref="D40:AD40" si="1">SUM(D2:D39)</f>
+      <c r="E40">
+        <f t="shared" ref="E40:AE40" si="2">SUM(E2:E39)</f>
         <v>902</v>
       </c>
-      <c r="E40">
-        <f t="shared" si="1"/>
+      <c r="F40">
+        <f t="shared" si="2"/>
         <v>328</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
+      <c r="G40">
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
-      <c r="G40">
-        <f t="shared" si="1"/>
+      <c r="H40">
+        <f t="shared" si="2"/>
         <v>942</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="1"/>
+      <c r="I40">
+        <f t="shared" si="2"/>
         <v>699</v>
       </c>
-      <c r="I40">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
       <c r="J40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="1"/>
+      <c r="L40">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="L40">
-        <f t="shared" si="1"/>
+      <c r="M40">
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
-      <c r="M40">
-        <f t="shared" si="1"/>
+      <c r="N40">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="N40">
-        <f t="shared" si="1"/>
+      <c r="O40">
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="O40">
-        <f t="shared" si="1"/>
+      <c r="P40">
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="1"/>
+      <c r="Q40">
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="Q40">
-        <f t="shared" si="1"/>
+      <c r="R40">
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
-      <c r="R40">
-        <f t="shared" si="1"/>
+      <c r="S40">
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="S40">
-        <f t="shared" si="1"/>
+      <c r="T40">
+        <f t="shared" si="2"/>
         <v>205</v>
       </c>
-      <c r="T40">
-        <f t="shared" si="1"/>
+      <c r="U40">
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="U40">
-        <f t="shared" si="1"/>
+      <c r="V40">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="V40">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="W40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="X40">
-        <f t="shared" si="1"/>
+      <c r="Y40">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="Y40">
-        <f t="shared" si="1"/>
+      <c r="Z40">
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="Z40">
-        <f t="shared" si="1"/>
+      <c r="AA40">
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="AA40">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="AB40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="AC40">
-        <f t="shared" si="1"/>
+      <c r="AD40">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AD40">
-        <f t="shared" si="1"/>
+      <c r="AE40">
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6 move symbols included
</commit_message>
<xml_diff>
--- a/file-statistics.xlsx
+++ b/file-statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\TU Darmstadt\Masterarbeit\chess-annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F4BB75-20DE-4649-A4A3-5A2AF4E03606}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4326E4EA-6461-4690-87F1-DA9267399356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CB797301-E421-4290-AD9C-F33B313D1461}"/>
   </bookViews>
@@ -198,6 +198,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{5D759E09-863F-4AAD-935E-A85986E9D127}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A15" authorId="0" shapeId="0" xr:uid="{14F7E778-DACF-4C1A-B94B-D2D3A8D7C6D5}">
       <text>
         <r>
@@ -219,6 +243,30 @@
           </rPr>
           <t xml:space="preserve">
 multiple languages</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{F8A1296C-FDC2-4371-967C-F06B9E2272A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florian Beck:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+it</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
top words list fixed, class mapping added and old print statements deleted
</commit_message>
<xml_diff>
--- a/file-statistics.xlsx
+++ b/file-statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\TU Darmstadt\Masterarbeit\chess-annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4326E4EA-6461-4690-87F1-DA9267399356}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EC3141-B057-4DCC-B693-259FCD3CEEA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CB797301-E421-4290-AD9C-F33B313D1461}"/>
   </bookViews>
@@ -1160,25 +1160,25 @@
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1352,22 +1352,22 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1736,13 +1736,13 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1751,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1928,25 +1928,25 @@
       </c>
       <c r="C11">
         <f t="shared" ref="C11:C39" si="1">SUM(D11:AE11)</f>
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="D11">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E11">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2024,19 +2024,19 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2120,25 +2120,25 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="D13">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="E13">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I13">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2216,19 +2216,19 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="D14">
         <v>69</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F14">
         <v>15</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -4710,31 +4710,31 @@
       </c>
       <c r="C40">
         <f>SUM(C2:C39)</f>
-        <v>7482</v>
+        <v>7858</v>
       </c>
       <c r="D40">
         <f>SUM(D2:D39)</f>
-        <v>3225</v>
+        <v>3375</v>
       </c>
       <c r="E40">
         <f t="shared" ref="E40:AE40" si="2">SUM(E2:E39)</f>
-        <v>902</v>
+        <v>999</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="G40">
         <f t="shared" si="2"/>
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>942</v>
+        <v>975</v>
       </c>
       <c r="I40">
         <f t="shared" si="2"/>
-        <v>699</v>
+        <v>752</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
first tests of naivebayes and decisiontree classifier with reduced data set
</commit_message>
<xml_diff>
--- a/file-statistics.xlsx
+++ b/file-statistics.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\TU Darmstadt\Masterarbeit\chess-annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Documents\TU Darmstadt\Masterarbeit\chess-annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EC3141-B057-4DCC-B693-259FCD3CEEA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD75870-C00A-4AE0-8C22-716DD2CB409F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CB797301-E421-4290-AD9C-F33B313D1461}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4470" xr2:uid="{CB797301-E421-4290-AD9C-F33B313D1461}"/>
   </bookViews>
   <sheets>
     <sheet name="all-classes" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -275,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>files/bali02.pgn</t>
   </si>
@@ -482,6 +487,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>"+/- ratio"</t>
   </si>
 </sst>
 </file>
@@ -536,7 +544,11 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -550,9 +562,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7184EF4-25C3-4BC2-8006-D03EA3E4CADA}" name="Tabelle4" displayName="Tabelle4" ref="A1:AE40" totalsRowCount="1">
-  <autoFilter ref="A1:AE39" xr:uid="{CF6BAA34-CBCC-4959-B3F2-DD4EC0EA728D}"/>
-  <tableColumns count="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7184EF4-25C3-4BC2-8006-D03EA3E4CADA}" name="Tabelle4" displayName="Tabelle4" ref="A1:AF40" totalsRowCount="1">
+  <autoFilter ref="A1:AF39" xr:uid="{CF6BAA34-CBCC-4959-B3F2-DD4EC0EA728D}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{E6C94211-23A1-4145-A10C-FC15029287A1}" name="File"/>
     <tableColumn id="31" xr3:uid="{F174BBBB-376E-4106-BA42-E7CF2824B6B0}" name="Comments" totalsRowFunction="custom">
       <totalsRowFormula>SUM(B2:B39)</totalsRowFormula>
@@ -644,6 +656,9 @@
     </tableColumn>
     <tableColumn id="30" xr3:uid="{F962C768-4B69-4ACA-ABB5-B35A21282D38}" name="146" totalsRowFunction="custom">
       <totalsRowFormula>SUM(AE2:AE39)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="32" xr3:uid="{5E379837-FDF6-4D04-A62E-79840425BBDD}" name="&quot;+/- ratio&quot;" dataDxfId="0">
+      <calculatedColumnFormula>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -947,20 +962,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2754611A-D4BC-4997-8208-F8CC3E0865F3}">
-  <dimension ref="A1:AE40"/>
+  <dimension ref="A1:AF40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" customWidth="1"/>
-    <col min="4" max="26" width="5.140625" customWidth="1"/>
-    <col min="27" max="31" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" customWidth="1"/>
+    <col min="4" max="26" width="5.1796875" customWidth="1"/>
+    <col min="27" max="31" width="6.1796875" customWidth="1"/>
+    <col min="32" max="32" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1054,8 +1072,11 @@
       <c r="AE1" t="s">
         <v>48</v>
       </c>
+      <c r="AF1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1150,8 +1171,12 @@
       <c r="AE2">
         <v>0</v>
       </c>
+      <c r="AF2">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.1538461538461537</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1246,8 +1271,12 @@
       <c r="AE3">
         <v>0</v>
       </c>
+      <c r="AF3">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>0.46153846153846156</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1342,8 +1371,12 @@
       <c r="AE4">
         <v>0</v>
       </c>
+      <c r="AF4">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1438,8 +1471,12 @@
       <c r="AE5">
         <v>0</v>
       </c>
+      <c r="AF5">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1534,8 +1571,12 @@
       <c r="AE6">
         <v>0</v>
       </c>
+      <c r="AF6">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.2826086956521738</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1630,8 +1671,12 @@
       <c r="AE7">
         <v>0</v>
       </c>
+      <c r="AF7">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1726,8 +1771,12 @@
       <c r="AE8">
         <v>0</v>
       </c>
+      <c r="AF8">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1822,8 +1871,12 @@
       <c r="AE9">
         <v>0</v>
       </c>
+      <c r="AF9">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>2.9310344827586206</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1918,8 +1971,12 @@
       <c r="AE10">
         <v>0</v>
       </c>
+      <c r="AF10">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.3076923076923075</v>
+      </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2014,8 +2071,12 @@
       <c r="AE11">
         <v>0</v>
       </c>
+      <c r="AF11">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2110,8 +2171,12 @@
       <c r="AE12">
         <v>0</v>
       </c>
+      <c r="AF12">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.3333333333333333</v>
+      </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2206,8 +2271,12 @@
       <c r="AE13">
         <v>2</v>
       </c>
+      <c r="AF13">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.8378378378378379</v>
+      </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2302,8 +2371,12 @@
       <c r="AE14">
         <v>0</v>
       </c>
+      <c r="AF14">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>2.5294117647058822</v>
+      </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2398,8 +2471,12 @@
       <c r="AE15">
         <v>1</v>
       </c>
+      <c r="AF15">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>4.3663366336633667</v>
+      </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2494,8 +2571,12 @@
       <c r="AE16">
         <v>0</v>
       </c>
+      <c r="AF16">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2590,8 +2671,12 @@
       <c r="AE17">
         <v>0</v>
       </c>
+      <c r="AF17">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2686,8 +2771,12 @@
       <c r="AE18">
         <v>0</v>
       </c>
+      <c r="AF18">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>0.91666666666666663</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2782,8 +2871,12 @@
       <c r="AE19">
         <v>4</v>
       </c>
+      <c r="AF19">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>27.5</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2878,8 +2971,12 @@
       <c r="AE20">
         <v>1</v>
       </c>
+      <c r="AF20">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.2051282051282051</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2974,8 +3071,12 @@
       <c r="AE21">
         <v>0</v>
       </c>
+      <c r="AF21">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>4.1401273885350323</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3070,8 +3171,12 @@
       <c r="AE22">
         <v>0</v>
       </c>
+      <c r="AF22">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>4.2142857142857144</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3166,8 +3271,12 @@
       <c r="AE23">
         <v>0</v>
       </c>
+      <c r="AF23">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3262,8 +3371,12 @@
       <c r="AE24">
         <v>0</v>
       </c>
+      <c r="AF24">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.3695652173913042</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3358,8 +3471,12 @@
       <c r="AE25">
         <v>0</v>
       </c>
+      <c r="AF25">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>0.95238095238095233</v>
+      </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3454,8 +3571,12 @@
       <c r="AE26">
         <v>1</v>
       </c>
+      <c r="AF26">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.125</v>
+      </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3550,8 +3671,12 @@
       <c r="AE27">
         <v>0</v>
       </c>
+      <c r="AF27">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3646,8 +3771,12 @@
       <c r="AE28">
         <v>1</v>
       </c>
+      <c r="AF28">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3742,8 +3871,12 @@
       <c r="AE29">
         <v>12</v>
       </c>
+      <c r="AF29">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>4.7692307692307692</v>
+      </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3838,8 +3971,12 @@
       <c r="AE30">
         <v>1</v>
       </c>
+      <c r="AF30">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.6716417910447761</v>
+      </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3934,8 +4071,12 @@
       <c r="AE31">
         <v>0</v>
       </c>
+      <c r="AF31">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>55</v>
+      </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -4030,8 +4171,12 @@
       <c r="AE32">
         <v>0</v>
       </c>
+      <c r="AF32">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -4126,8 +4271,12 @@
       <c r="AE33">
         <v>0</v>
       </c>
+      <c r="AF33">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.1818181818181819</v>
+      </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -4222,8 +4371,12 @@
       <c r="AE34">
         <v>2</v>
       </c>
+      <c r="AF34">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.875</v>
+      </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -4318,8 +4471,12 @@
       <c r="AE35">
         <v>3</v>
       </c>
+      <c r="AF35">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>4.1851851851851851</v>
+      </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -4414,8 +4571,12 @@
       <c r="AE36">
         <v>0</v>
       </c>
+      <c r="AF36">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>5.375</v>
+      </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -4510,8 +4671,12 @@
       <c r="AE37">
         <v>0</v>
       </c>
+      <c r="AF37">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>1.6875</v>
+      </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -4606,8 +4771,12 @@
       <c r="AE38">
         <v>0</v>
       </c>
+      <c r="AF38">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4702,8 +4871,12 @@
       <c r="AE39">
         <v>0</v>
       </c>
+      <c r="AF39">
+        <f>(Tabelle4[[#This Row],[1]]+Tabelle4[[#This Row],[3]]+Tabelle4[[#This Row],[5]]+1)/(Tabelle4[[#This Row],[2]]+Tabelle4[[#This Row],[4]]+Tabelle4[[#This Row],[6]]+1)</f>
+        <v>2.9088785046728973</v>
+      </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B40">
         <f>SUM(B2:B39)</f>
         <v>50762</v>

</xml_diff>